<commit_message>
v1.1 via stitching added
</commit_message>
<xml_diff>
--- a/Project Outputs/BOM/Bill of Materials-BOM.xlsx
+++ b/Project Outputs/BOM/Bill of Materials-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\RCL\POWER-CONNECTOR\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0414E19B-2F72-498F-8AC2-EFA767AA064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B73777-C0DD-4F8B-919D-2BD255D7242A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{3B441423-FD93-4901-9D17-E7CE4BA55193}"/>
+    <workbookView xWindow="6195" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{70FAB241-C7D4-4083-8784-7FDA20703262}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Designator</t>
   </si>
@@ -108,13 +108,10 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>502494-0670</t>
+    <t>502585-0670</t>
   </si>
   <si>
     <t>1.50mm Pitch, CLIK-Mate PCB Receptacle, Single Row, Surface Mount, Right-Angle, Tin Plating, Positive Lock, 6 Circuits, Natural</t>
-  </si>
-  <si>
-    <t>502585-0670</t>
   </si>
   <si>
     <t>IN</t>
@@ -503,7 +500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB670C81-EEE8-4D7F-90E0-76F7D456AE37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228B3DFA-8CC2-4F7F-A0A7-CCA0D9EFC423}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -621,25 +618,25 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>15</v>
@@ -649,7 +646,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>